<commit_message>
created report, finished eda
#8 #2
</commit_message>
<xml_diff>
--- a/doc/Bewertungskrieterien.xlsx
+++ b/doc/Bewertungskrieterien.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sandra\Documents\GitHub\wdb_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sandra\Documents\GitHub\wdb_webscraping\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16CB2ED7-3FA9-4A07-88EB-9D122214C1C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2064365-E754-40E0-860E-6C0D147322DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
   <si>
     <t>Description</t>
   </si>
@@ -173,12 +173,231 @@
   <si>
     <t>Adi</t>
   </si>
+  <si>
+    <t>die y.XPATH, "//button[.//span[text()='Mehr anzeigen'] als variabkle am anfang des codes</t>
+  </si>
+  <si>
+    <t>die exeptions besser prüfen und mehr integrieren</t>
+  </si>
+  <si>
+    <r>
+      <t>except</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FFCAD3F5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="7"/>
+        <color rgb="FFC6A0F6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Exception</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FFCAD3F5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FFC6A0F6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>as</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FFCAD3F5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> e</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF939AB7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FFEED49F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>logging</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF939AB7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="7"/>
+        <color rgb="FF8AADF4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>error</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF939AB7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="7"/>
+        <color rgb="FFA6DA95"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FFA6DA95"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">"Fehler beim Laden der Frontpage: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FFF5BDE6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FFCAD3F5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>e</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FFF5BDE6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FFA6DA95"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF939AB7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">            attempts </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF8BD5CA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>+=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FFCAD3F5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FFF5A97F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <t>Michelle, läuft ab python 3.12</t>
+  </si>
+  <si>
+    <t>https://sphinxcontrib-napoleon.readthedocs.io/en/latest/example_google.html</t>
+  </si>
+  <si>
+    <t>adi</t>
+  </si>
+  <si>
+    <t>loggin, ü komisch, in utf8 speichern - Sa</t>
+  </si>
+  <si>
+    <t>docstrings nach google docstrings machen michelle</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,6 +438,82 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FFCAD3F5"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FFC6A0F6"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="7"/>
+      <color rgb="FFC6A0F6"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF939AB7"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FFEED49F"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="7"/>
+      <color rgb="FF8AADF4"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="7"/>
+      <color rgb="FFA6DA95"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FFA6DA95"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FFF5BDE6"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF8BD5CA"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FFF5A97F"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -379,7 +674,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -419,6 +714,19 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -813,10 +1121,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="138" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="138" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -827,7 +1135,7 @@
     <col min="6" max="6" width="72.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="8" t="s">
@@ -843,34 +1151,34 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="18"/>
       <c r="B2" s="13">
         <v>1</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="35"/>
-    </row>
-    <row r="3" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="21"/>
-      <c r="C3" s="23" t="s">
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="44"/>
+    </row>
+    <row r="3" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="35"/>
+      <c r="C3" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="38">
         <v>10</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3" s="39">
         <v>10</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="39" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="18"/>
       <c r="C4" s="6" t="s">
         <v>30</v>
@@ -883,7 +1191,7 @@
       </c>
       <c r="F4" s="10"/>
     </row>
-    <row r="5" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="21"/>
       <c r="C5" s="23" t="s">
         <v>6</v>
@@ -894,21 +1202,26 @@
       <c r="E5" s="25">
         <v>5</v>
       </c>
-      <c r="F5" s="25"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F5" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="18"/>
       <c r="B6" s="4">
         <v>2</v>
       </c>
-      <c r="C6" s="43" t="s">
+      <c r="C6" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="45"/>
-    </row>
-    <row r="7" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="54"/>
+    </row>
+    <row r="7" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="26"/>
       <c r="C7" s="23" t="s">
         <v>8</v>
@@ -923,19 +1236,19 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="18"/>
       <c r="B8" s="4">
         <v>3</v>
       </c>
-      <c r="C8" s="50" t="s">
+      <c r="C8" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="52"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D8" s="60"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="61"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="18"/>
       <c r="C9" s="6" t="s">
         <v>31</v>
@@ -946,9 +1259,14 @@
       <c r="E9" s="10">
         <v>5</v>
       </c>
-      <c r="F9" s="10"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F9" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="33" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="18"/>
       <c r="C10" s="6" t="s">
         <v>33</v>
@@ -959,9 +1277,14 @@
       <c r="E10" s="10">
         <v>5</v>
       </c>
-      <c r="F10" s="10"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F10" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="18"/>
       <c r="C11" s="6" t="s">
         <v>10</v>
@@ -973,20 +1296,23 @@
         <v>5</v>
       </c>
       <c r="F11" s="10"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G11" s="34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="18"/>
       <c r="B12" s="4">
         <v>4</v>
       </c>
-      <c r="C12" s="43" t="s">
+      <c r="C12" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="45"/>
-    </row>
-    <row r="13" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="54"/>
+    </row>
+    <row r="13" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="30"/>
       <c r="C13" s="32" t="s">
         <v>34</v>
@@ -998,10 +1324,10 @@
         <v>0</v>
       </c>
       <c r="F13" s="29" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="18"/>
       <c r="C14" s="6" t="s">
         <v>12</v>
@@ -1012,9 +1338,14 @@
       <c r="E14" s="10">
         <v>5</v>
       </c>
-      <c r="F14" s="10"/>
-    </row>
-    <row r="15" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F14" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="26"/>
       <c r="C15" s="23" t="s">
         <v>13</v>
@@ -1029,45 +1360,45 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="18"/>
       <c r="B16" s="4">
         <v>5</v>
       </c>
-      <c r="C16" s="43" t="s">
+      <c r="C16" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="44"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="45"/>
-    </row>
-    <row r="17" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="26"/>
-      <c r="C17" s="23" t="s">
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="54"/>
+    </row>
+    <row r="17" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="30"/>
+      <c r="C17" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="28">
+      <c r="D17" s="40">
         <v>5</v>
       </c>
-      <c r="E17" s="29">
+      <c r="E17" s="41">
         <v>0</v>
       </c>
-      <c r="F17" s="29" t="s">
+      <c r="F17" s="41" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="26"/>
-      <c r="C18" s="23" t="s">
+    <row r="18" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="30"/>
+      <c r="C18" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="28">
+      <c r="D18" s="40">
         <v>5</v>
       </c>
-      <c r="E18" s="29">
+      <c r="E18" s="41">
         <v>0</v>
       </c>
-      <c r="F18" s="29" t="s">
+      <c r="F18" s="41" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1076,12 +1407,12 @@
       <c r="B19" s="4">
         <v>6</v>
       </c>
-      <c r="C19" s="43" t="s">
+      <c r="C19" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="44"/>
-      <c r="E19" s="44"/>
-      <c r="F19" s="45"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="54"/>
     </row>
     <row r="20" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="26"/>
@@ -1144,12 +1475,12 @@
       <c r="B24" s="4">
         <v>7</v>
       </c>
-      <c r="C24" s="43" t="s">
+      <c r="C24" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="44"/>
-      <c r="E24" s="44"/>
-      <c r="F24" s="45"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="54"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="18"/>
@@ -1167,12 +1498,12 @@
       <c r="B26" s="4">
         <v>8</v>
       </c>
-      <c r="C26" s="43" t="s">
+      <c r="C26" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="44"/>
-      <c r="E26" s="44"/>
-      <c r="F26" s="45"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="54"/>
     </row>
     <row r="27" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="26"/>
@@ -1194,12 +1525,12 @@
       <c r="B28" s="5">
         <v>9</v>
       </c>
-      <c r="C28" s="40" t="s">
+      <c r="C28" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="42"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="51"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="18"/>
@@ -1219,37 +1550,37 @@
       <c r="A30" s="18"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="46"/>
-      <c r="E30" s="47"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="56"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="18"/>
       <c r="C31" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D31" s="36">
+      <c r="D31" s="45">
         <f>SUM(D3:D23)</f>
         <v>100</v>
       </c>
-      <c r="E31" s="37"/>
+      <c r="E31" s="46"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="18"/>
       <c r="C32" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D32" s="36">
+      <c r="D32" s="45">
         <f>SUM(E3:E23)*E25+E27+E29</f>
         <v>44</v>
       </c>
-      <c r="E32" s="37"/>
+      <c r="E32" s="46"/>
     </row>
     <row r="33" spans="1:5" ht="7.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="18"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
-      <c r="D33" s="48"/>
-      <c r="E33" s="49"/>
+      <c r="D33" s="57"/>
+      <c r="E33" s="58"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="19"/>
@@ -1257,11 +1588,11 @@
       <c r="C34" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D34" s="38">
+      <c r="D34" s="47">
         <f>MAX(1,MIN(6,1+(D32/D31)*5))</f>
         <v>3.2</v>
       </c>
-      <c r="E34" s="39"/>
+      <c r="E34" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -1286,12 +1617,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100E044C053010459458C1BC44D0C44A23D" ma:contentTypeVersion="4" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="ee773e2e89ac35d6137e0e25a2cf1843">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f6e58a51-fb8f-40ff-9ca4-111825cddd76" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5e4daf0e4151dc6f77d59c5239c42fa6" ns2:_="">
     <xsd:import namespace="f6e58a51-fb8f-40ff-9ca4-111825cddd76"/>
@@ -1435,16 +1775,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53FD9FDE-2A6C-4C35-90CD-B15322751343}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA86D45E-F4F5-4E44-AA29-60F8D1369878}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1453,7 +1792,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6BF3A3A-CFC7-4120-8D43-C5F0A555D866}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1469,12 +1808,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53FD9FDE-2A6C-4C35-90CD-B15322751343}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>